<commit_message>
Overhaul / Version 3 (#10)
There are a lot of breaking changes in v3:

- The JSON Spreadsheet format (JSF) has been cleaned up, made more
internally consistent, and speced out (at least the parts this converter
uses).
  - All properties and values are camelCased.
  - All units are now pixels (closes #5)
- Some things (cell props) made more consistent with original CSF spec.
- The project has been converted to TypeScript.
- All dependencies updated.
- The workbook object is no longer used as a storage during conversion.
- Options redone:
  - Option props now use camelCase.
  - Removed cell_styles and cell_z options.
- Added a cellFormulas option. Cell formulas are not deduplicated by
default, as this reduces the files dramatically. But It makes sense to
allow emitting the A1 versions on cells as well.
</commit_message>
<xml_diff>
--- a/tests/files/table.xlsx
+++ b/tests/files/table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10516"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11016"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borgar/Sites/borgar-github/xlsx-convert/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4337C67-7FB0-E94F-8D00-D807FCDE2B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74B16EC-AC32-B240-BB09-10E050739541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10820" yWindow="500" windowWidth="29160" windowHeight="27080" xr2:uid="{8F98B8F1-5C91-9649-BF3F-F56BE376E84A}"/>
+    <workbookView xWindow="1960" yWindow="2320" windowWidth="28860" windowHeight="24800" activeTab="1" xr2:uid="{8F98B8F1-5C91-9649-BF3F-F56BE376E84A}"/>
   </bookViews>
   <sheets>
     <sheet name="Pokémon" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="191">
   <si>
     <t>Index #</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>BMI class</t>
+  </si>
+  <si>
+    <t>Headers are hidden</t>
   </si>
 </sst>
 </file>
@@ -614,7 +617,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -654,12 +657,18 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -674,12 +683,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="0.0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -710,15 +713,15 @@
     <tableColumn id="5" xr3:uid="{3BBEF293-8DA9-B84C-90BF-FD4CF217C2B7}" name="Sec. Type" totalsRowFunction="custom">
       <totalsRowFormula>COUNTA(_xlfn.UNIQUE(Table1[Sec. Type]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{103C7433-6BFD-3647-8524-A8BF3C5E64BF}" name="Hp" totalsRowFunction="average" totalsRowDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{58265730-727D-C244-AB2D-887619C1EB47}" name="Catch rate" totalsRowFunction="average" totalsRowDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{535269B2-3A33-3C41-A7F9-3DF16A53E137}" name="Speed" totalsRowFunction="count" totalsRowDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{15ED5E07-4285-AE4F-BD6B-38E66E972FE7}" name="Weight (k)" totalsRowFunction="average" totalsRowDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{06B06D61-E11F-AB47-98DB-E6D52969D5DC}" name="Height (cm)" totalsRowFunction="average" totalsRowDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{AD16C30F-F543-E94A-ABDC-CEC0D421278B}" name="BMI" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{103C7433-6BFD-3647-8524-A8BF3C5E64BF}" name="Hp" totalsRowFunction="average" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{58265730-727D-C244-AB2D-887619C1EB47}" name="Catch rate" totalsRowFunction="average" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{535269B2-3A33-3C41-A7F9-3DF16A53E137}" name="Speed" totalsRowFunction="count" totalsRowDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{15ED5E07-4285-AE4F-BD6B-38E66E972FE7}" name="Weight (k)" totalsRowFunction="average" totalsRowDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{06B06D61-E11F-AB47-98DB-E6D52969D5DC}" name="Height (cm)" totalsRowFunction="average" totalsRowDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{AD16C30F-F543-E94A-ABDC-CEC0D421278B}" name="BMI" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[Weight (k)]]/((Table1[[#This Row],[Height (cm)]]/100)^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{50A83C02-B629-7946-BA4B-4B300E3DF44B}" name="BMI class" dataDxfId="5">
+    <tableColumn id="14" xr3:uid="{50A83C02-B629-7946-BA4B-4B300E3DF44B}" name="BMI class" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[BMI]],BMI[Min],BMI[Status],,-1,1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -727,25 +730,63 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2876AC68-F78A-5943-AB0F-139E2DDA173D}" name="BMI" displayName="BMI" ref="A1:C7" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2876AC68-F78A-5943-AB0F-139E2DDA173D}" name="BMI" displayName="BMI" ref="A1:C8" totalsRowCount="1">
   <autoFilter ref="A1:C7" xr:uid="{2876AC68-F78A-5943-AB0F-139E2DDA173D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{68945EC9-0629-0745-9EBD-7B416B4EBFE0}" name="Min"/>
-    <tableColumn id="2" xr3:uid="{0D8027E7-572B-7B44-97C7-BD3F1549331F}" name="Max"/>
-    <tableColumn id="3" xr3:uid="{2071F3C1-CA97-CA4A-B00B-08EBF4BC5EAD}" name="Status"/>
+    <tableColumn id="1" xr3:uid="{68945EC9-0629-0745-9EBD-7B416B4EBFE0}" name="Min" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{0D8027E7-572B-7B44-97C7-BD3F1549331F}" name="Max" totalsRowFunction="var"/>
+    <tableColumn id="3" xr3:uid="{2071F3C1-CA97-CA4A-B00B-08EBF4BC5EAD}" name="Status" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="This is the alt text"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6201CC35-62B4-DA46-A335-3D8D60864C36}" name="BMI_5" displayName="BMI_5" ref="A11:C17">
+  <autoFilter ref="A11:C17" xr:uid="{6201CC35-62B4-DA46-A335-3D8D60864C36}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E538E853-130F-3740-8743-C073D13773E8}" name="Min" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{038CF476-11F4-5F4F-9A07-5FD6D8D9851F}" name="Max" totalsRowFunction="var"/>
+    <tableColumn id="3" xr3:uid="{BD98347E-F00C-BF48-A5B8-F10063F0ACAF}" name="Status" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="This is the alt text"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5FD315B2-92F0-C241-A942-9364572FD0DB}" name="BMI_6" displayName="BMI_6" ref="A21:C26" headerRowCount="0">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{85AAAB1F-4C30-B146-9055-3C0ECEF74DDB}" name="Min" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{72DA0635-B5A0-6644-893B-B50DD0DCE209}" name="Max" totalsRowFunction="var"/>
+    <tableColumn id="3" xr3:uid="{17123947-7608-544B-9B80-C9153A32565A}" name="Status" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="This is the alt text"/>
+    </ext>
+  </extLst>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -783,7 +824,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -889,7 +930,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1031,7 +1072,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1041,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60F22FD-5A5D-1647-A706-23CCAADE2A30}">
   <dimension ref="A1:L153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6927,10 +6968,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E6FA35-D670-4F44-8441-57CEE261A654}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7015,11 +7056,174 @@
         <v>188</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8">
+        <f>SUBTOTAL(110,BMI[Max])</f>
+        <v>16567870.041666666</v>
+      </c>
+      <c r="C8">
+        <f>SUBTOTAL(103,BMI[Status])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>18.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>18.5</v>
+      </c>
+      <c r="B13">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>10000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>18.5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>18.5</v>
+      </c>
+      <c r="B22">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>10000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add spec and support for table styles
The new properties have been used directly from the xlsx spec.
</commit_message>
<xml_diff>
--- a/tests/files/table.xlsx
+++ b/tests/files/table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11016"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borgar/Sites/borgar-github/xlsx-convert/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74B16EC-AC32-B240-BB09-10E050739541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A800D33-E4C9-7C4E-8A0A-C18DFCA00DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="2320" windowWidth="28860" windowHeight="24800" activeTab="1" xr2:uid="{8F98B8F1-5C91-9649-BF3F-F56BE376E84A}"/>
   </bookViews>
@@ -752,7 +752,11 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6201CC35-62B4-DA46-A335-3D8D60864C36}" name="BMI_5" displayName="BMI_5" ref="A11:C17">
-  <autoFilter ref="A11:C17" xr:uid="{6201CC35-62B4-DA46-A335-3D8D60864C36}"/>
+  <autoFilter ref="A11:C17" xr:uid="{6201CC35-62B4-DA46-A335-3D8D60864C36}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E538E853-130F-3740-8743-C073D13773E8}" name="Min" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{038CF476-11F4-5F4F-9A07-5FD6D8D9851F}" name="Max" totalsRowFunction="var"/>
@@ -6971,7 +6975,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>